<commit_message>
fixed function bounder in hw2 and update excel
</commit_message>
<xml_diff>
--- a/580610616_hw1_1_2.xlsx
+++ b/580610616_hw1_1_2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="hw1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="82">
   <si>
     <t>mid</t>
   </si>
@@ -234,36 +234,6 @@
     <t>12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 28.0</t>
   </si>
   <si>
-    <t>0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.04, 0.04, 0.04, 0.04, 0.04, 0.08, 0.085, 0.125, 0.125, 0.125, 0.125, 0.125, 0.165, 0.165, 0.165, 0.165, 0.165, 0.165, 0.165, 0.165, 0.17, 0.205, 0.205, 0.205, 0.21, 0.21, 0.21, 0.25, 0.25, 0.25, 0.25, 0.25, 0.25, 0.29, 0.29, 0.29, 0.29, 0.29, 0.29, 0.335, 0.335, 0.335, 0.335, 0.335, 0.335, 0.375, 0.375, 0.375, 0.375, 0.375</t>
-  </si>
-  <si>
-    <t>0.375, 0.375, 0.375, 0.375, 0.415, 0.415, 0.415, 0.415, 0.42, 0.42, 0.46, 0.46, 0.46, 0.46, 0.5, 0.5, 0.5, 0.5, 0.5, 0.5, 0.5, 0.5, 0.5, 0.5, 0.5, 0.5, 0.5, 0.5, 0.5, 0.54, 0.54, 0.54, 0.54, 0.54, 0.54, 0.54, 0.54, 0.58, 0.58, 0.585, 0.585, 0.585, 0.585, 0.585, 0.585, 0.585, 0.585, 0.585, 0.585, 0.625, 0.625, 0.625, 0.665, 0.665, 0.665, 0.665, 0.67, 0.705, 0.71, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75</t>
-  </si>
-  <si>
-    <t>0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.79, 0.79, 0.79, 0.79, 0.83, 0.83, 0.83, 0.835, 0.835, 0.835, 0.835, 0.835, 0.835, 0.835, 0.835, 0.875, 0.875, 0.875, 0.875, 0.875, 0.875, 0.915, 0.96, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.0, 1.04, 1.04, 1.04, 1.04, 1.04, 1.04, 1.08, 1.085, 1.085, 1.085, 1.125, 1.125, 1.125, 1.125, 1.165, 1.165, 1.21, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25</t>
-  </si>
-  <si>
-    <t>1.25, 1.25, 1.25, 1.29, 1.335, 1.335, 1.335, 1.375, 1.375, 1.415, 1.46, 1.5, 1.5, 1.5, 1.5, 1.5, 1.5, 1.5, 1.5, 1.5, 1.5, 1.5, 1.5, 1.5, 1.5, 1.5, 1.5, 1.5, 1.5, 1.5, 1.5, 1.5, 1.54, 1.54, 1.54, 1.54, 1.54, 1.54, 1.585, 1.585, 1.585, 1.585, 1.625, 1.625, 1.625, 1.665, 1.665, 1.665, 1.665, 1.71, 1.71, 1.71, 1.75, 1.75, 1.75, 1.75, 1.75, 1.75, 1.75, 1.75, 1.75, 1.75, 1.75, 1.75, 1.79, 1.835, 1.835, 1.835, 1.835</t>
-  </si>
-  <si>
-    <t>2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.04, 2.04, 2.04, 2.04, 2.04, 2.04, 2.085, 2.085, 2.125, 2.165, 2.165, 2.21, 2.25, 2.25, 2.25, 2.25, 2.25, 2.29, 2.29, 2.335, 2.335, 2.335, 2.415, 2.415, 2.415, 2.46, 2.5, 2.5, 2.5, 2.5, 2.5, 2.5, 2.5, 2.5, 2.5, 2.5, 2.5, 2.5, 2.5, 2.5, 2.5, 2.5, 2.5, 2.5, 2.5, 2.54, 2.54, 2.54, 2.54, 2.665, 2.71, 2.71, 2.71, 2.71, 2.75, 2.75, 2.75, 2.75, 2.75</t>
-  </si>
-  <si>
-    <t>2.75, 2.75, 2.835, 2.875, 2.875, 3.0, 3.0, 3.0, 3.0, 3.0, 3.0, 3.0, 3.0, 3.0, 3.0, 3.0, 3.0, 3.0, 3.0, 3.0, 3.0, 3.0, 3.0, 3.0, 3.04, 3.04, 3.085, 3.125, 3.125, 3.165, 3.165, 3.165, 3.165, 3.25, 3.25, 3.25, 3.29, 3.29, 3.335, 3.375, 3.5, 3.5, 3.5, 3.5, 3.5, 3.5, 3.5, 3.5, 3.54, 3.54, 3.625, 3.75, 3.75, 3.75, 3.75, 3.75, 3.79, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0</t>
-  </si>
-  <si>
-    <t>4.04, 4.04, 4.085, 4.085, 4.125, 4.165, 4.25, 4.25, 4.25, 4.25, 4.25, 4.25, 4.415, 4.415, 4.415, 4.46, 4.46, 4.46, 4.5, 4.5, 4.5, 4.5, 4.5, 4.585, 4.625, 4.625, 4.71, 4.75, 4.79, 4.915, 5.0, 5.0, 5.0, 5.0, 5.0, 5.0, 5.0, 5.0, 5.0, 5.0, 5.0, 5.0, 5.0, 5.0, 5.04, 5.04, 5.085, 5.085, 5.125, 5.125, 5.25, 5.29, 5.29, 5.415, 5.5, 5.5, 5.5, 5.5, 5.5, 5.5, 5.5, 5.5, 5.625, 5.665, 5.71, 5.835, 5.875, 5.875, 6.0</t>
-  </si>
-  <si>
-    <t>6.0, 6.0, 6.0, 6.0, 6.0, 6.04, 6.165, 6.21, 6.5, 6.5, 6.5, 6.5, 6.5, 6.5, 6.5, 6.5, 6.5, 6.5, 6.5, 6.5, 6.625, 6.665, 6.75, 6.75, 7.0, 7.0, 7.0, 7.0, 7.0, 7.0, 7.0, 7.0, 7.04, 7.08, 7.25, 7.5, 7.5, 7.5, 7.5, 7.54, 7.585, 7.625, 7.625, 7.835, 8.0, 8.0, 8.125, 8.17, 8.46, 8.5, 8.5, 8.5, 8.5, 8.5, 8.585, 8.665, 9.0, 9.0, 9.0, 9.0, 9.0, 9.0, 9.0, 9.17, 9.25, 9.25, 9.25, 9.335, 9.415</t>
-  </si>
-  <si>
-    <t>9.5, 9.5, 9.5, 9.5, 9.5, 9.54, 9.54, 9.585, 9.625, 9.75, 9.79, 9.96, 10.0, 10.0, 10.0, 10.0, 10.0, 10.0, 10.0, 10.0, 10.0, 10.0, 10.04, 10.085, 10.125, 10.125, 10.21, 10.25, 10.25, 10.29, 10.335, 10.415, 10.5, 10.5, 10.5, 10.5, 10.5, 10.665, 10.75, 10.915, 11.0, 11.0, 11.0, 11.0, 11.0, 11.0, 11.0, 11.0, 11.0, 11.045, 11.125, 11.25, 11.25, 11.25, 11.46, 11.5, 11.5, 11.5, 11.5, 11.5, 11.5, 11.5, 11.5, 11.585, 11.625, 11.665, 11.75, 11.75, 11.835</t>
-  </si>
-  <si>
-    <t>12.0, 12.0, 12.0, 12.0, 12.0, 12.125, 12.25, 12.33, 12.335, 12.5, 12.5, 12.5, 12.5, 12.5, 12.5, 12.5, 12.5, 12.54, 12.625, 12.75, 12.75, 12.835, 13.0, 13.0, 13.0, 13.335, 13.5, 13.5, 13.5, 13.585, 13.665, 13.75, 13.915, 14.0, 14.0, 14.5, 14.5, 14.5, 14.585, 14.79, 15.0, 15.0, 15.0, 15.0, 15.0, 15.0, 15.5, 15.5, 16.0, 16.165, 16.5, 16.5, 17.75, 18.125, 18.5, 19.0, 19.0, 19.5, 19.5, 20.0, 21.0, 21.5, 22.0, 22.29, 25.085, 25.125, 25.21, 26.335, 28.0</t>
-  </si>
-  <si>
     <t>sum of frequcen</t>
   </si>
   <si>
@@ -274,13 +244,43 @@
   </si>
   <si>
     <t>จากกราฟก็จะเห็นว่าเบ้ซ้าน</t>
+  </si>
+  <si>
+    <t>0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375</t>
+  </si>
+  <si>
+    <t>0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.375, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75</t>
+  </si>
+  <si>
+    <t>0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 0.75, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25</t>
+  </si>
+  <si>
+    <t>1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.25, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835, 1.835</t>
+  </si>
+  <si>
+    <t>2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.0, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75</t>
+  </si>
+  <si>
+    <t>2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 2.75, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0, 4.0</t>
+  </si>
+  <si>
+    <t>4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 4.04, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0</t>
+  </si>
+  <si>
+    <t>6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 6.0, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415, 9.415</t>
+  </si>
+  <si>
+    <t>9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 9.5, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835, 11.835</t>
+  </si>
+  <si>
+    <t>12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 12.0, 28.0, 28.0, 28.0, 28.0, 28.0, 28.0, 28.0, 28.0, 28.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +309,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -318,7 +333,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -352,11 +367,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -376,6 +404,13 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,11 +557,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="773356960"/>
-        <c:axId val="773359440"/>
+        <c:axId val="-1432884656"/>
+        <c:axId val="-1465741440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="773356960"/>
+        <c:axId val="-1432884656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -569,7 +604,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="773359440"/>
+        <c:crossAx val="-1465741440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -577,7 +612,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="773359440"/>
+        <c:axId val="-1465741440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -627,7 +662,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="773356960"/>
+        <c:crossAx val="-1432884656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1543,7 +1578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
@@ -1571,7 +1606,7 @@
         <v>14</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>17</v>
@@ -1831,7 +1866,7 @@
     </row>
     <row r="38" spans="1:2" ht="21" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="21" x14ac:dyDescent="0.3">
@@ -1841,12 +1876,12 @@
     </row>
     <row r="40" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="B41" s="8" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1860,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2136,269 +2171,359 @@
         <v>690</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="21" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
+    <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>57</v>
       </c>
     </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>69</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>69</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33">
+        <v>69</v>
+      </c>
+      <c r="C33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>69</v>
+      </c>
+      <c r="C34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35">
+        <v>69</v>
+      </c>
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36">
+        <v>69</v>
+      </c>
+      <c r="C36" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>27</v>
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37">
+        <v>69</v>
+      </c>
+      <c r="C37" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B38">
         <v>69</v>
       </c>
       <c r="C38" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B39">
         <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <f>SUM(B30:B39)</f>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" s="11">
+        <v>69</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="11">
+        <v>69</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B40">
-        <v>69</v>
-      </c>
-      <c r="C40" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="B46" s="11">
+        <v>69</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B41">
-        <v>69</v>
-      </c>
-      <c r="C41" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B47" s="11">
+        <v>69</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B42">
-        <v>69</v>
-      </c>
-      <c r="C42" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="B48" s="11">
+        <v>69</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B43">
-        <v>69</v>
-      </c>
-      <c r="C43" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="B49" s="11">
+        <v>69</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B44">
-        <v>69</v>
-      </c>
-      <c r="C44" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="B50" s="11">
+        <v>69</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B45">
-        <v>69</v>
-      </c>
-      <c r="C45" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="B51" s="11">
+        <v>69</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B46">
-        <v>69</v>
-      </c>
-      <c r="C46" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="B52" s="11">
+        <v>69</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B47">
-        <v>69</v>
-      </c>
-      <c r="C47" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48">
-        <f>SUM(B38:B47)</f>
-        <v>690</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>28</v>
-      </c>
-      <c r="B51">
-        <v>69</v>
-      </c>
-      <c r="C51" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>30</v>
-      </c>
-      <c r="B52">
-        <v>69</v>
-      </c>
-      <c r="C52" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="B53" s="11">
+        <v>69</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B53">
-        <v>69</v>
-      </c>
-      <c r="C53" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="B54" s="11">
+        <v>69</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B54">
-        <v>69</v>
-      </c>
-      <c r="C54" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="B55" s="11">
+        <v>69</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B55">
-        <v>69</v>
-      </c>
-      <c r="C55" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="B56" s="11">
+        <v>69</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B56">
-        <v>69</v>
-      </c>
-      <c r="C56" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="B57" s="11">
+        <v>69</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B57">
-        <v>69</v>
-      </c>
-      <c r="C57" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="B58" s="11">
+        <v>69</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B58">
-        <v>69</v>
-      </c>
-      <c r="C58" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="B59" s="11">
+        <v>69</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B59">
-        <v>69</v>
-      </c>
-      <c r="C59" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="B60" s="11">
+        <v>69</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B60">
-        <v>69</v>
-      </c>
-      <c r="C60" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>1</v>
-      </c>
-      <c r="B61">
-        <f>SUM(B51:B60)</f>
-        <v>690</v>
+      <c r="B61" s="11">
+        <v>69</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>